<commit_message>
Missing Lines in ERP - Writing in Result Sheet
</commit_message>
<xml_diff>
--- a/Syteline_Extract_files/C0007259-NBF7259-Syteline Extract.xlsx
+++ b/Syteline_Extract_files/C0007259-NBF7259-Syteline Extract.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpadeveloper\Documents\UiPath\Fellowes_Validation\Syteline_Extract_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PragyanPattnaik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91C3FA8-A3FE-4081-BE70-263B5FD7BC61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3FBC1D0-C5E6-4862-8517-D9C676553886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" xr2:uid="{5E25725E-BB85-4D6E-9291-E770DD99163E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0FAEDC9F-582D-4E4C-8235-93E9B3ED62FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="77">
   <si>
     <t>SALES ORDER #</t>
   </si>
@@ -84,30 +84,132 @@
     <t>NBF7259</t>
   </si>
   <si>
+    <t>SIZRECT48STRCLMNBF</t>
+  </si>
+  <si>
+    <t>TOP;RECT;CLM;STR;48X48;NBF</t>
+  </si>
+  <si>
+    <t>FS SAWS A &amp; B</t>
+  </si>
+  <si>
+    <t>MATERIAL</t>
+  </si>
+  <si>
+    <t>810510-XZM</t>
+  </si>
+  <si>
+    <t>TFM;XZM;1.0X5X10-LIGHT GRAY</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>Work Instruction</t>
+  </si>
+  <si>
+    <t>A2 CUT 48.3960 X 48.3960  GRAIN 0CUT TO ROUGH SIZE</t>
+  </si>
+  <si>
+    <t>FS ROUTERS</t>
+  </si>
+  <si>
+    <t>FS EDGEBAND/BOX</t>
+  </si>
+  <si>
+    <t>(EXP)BLOCK;WS;SIDE FILLER</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>SEND TO 5209 FOR NBF PACKAGE LABEL</t>
+  </si>
+  <si>
+    <t>387880XZM</t>
+  </si>
+  <si>
+    <t>EDGEBAND;PVC;1.125X.118 IN;XZM</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>(EXP)BOX;TOP;WS;58.75 X 50.375 X 1.25</t>
+  </si>
+  <si>
+    <t>(EXP)BOX;BTM;WS;58.75 X 50.375 X 1.25</t>
+  </si>
+  <si>
+    <t>(EXP)END;BOX;WS;50.25 X 1.25 IN</t>
+  </si>
+  <si>
+    <t>LABEL;NBF;STICK ON</t>
+  </si>
+  <si>
+    <t>INTRINSIC ACCES/SERV</t>
+  </si>
+  <si>
+    <t>LABEL;PACKAGE;NBF;11 X 8.5</t>
+  </si>
+  <si>
+    <t>ATTACH NBF PACKAGE LABEL</t>
+  </si>
+  <si>
+    <t>PACK TABLES 99 PACK</t>
+  </si>
+  <si>
+    <t>CONNECTOR;TABLETOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>252794K</t>
+  </si>
+  <si>
+    <t>PLATE;SPPT;TABLE;6X3.5;K</t>
+  </si>
+  <si>
+    <t>KIT;HDWE;SCREW;BASE;TFL</t>
+  </si>
+  <si>
+    <t>SIZRECTSTRNBF</t>
+  </si>
+  <si>
+    <t>NBF40962;TABLE;RECT;STR;48X48</t>
+  </si>
+  <si>
+    <t>PARENT KNOCK DOWN WC</t>
+  </si>
+  <si>
+    <t>TKD</t>
+  </si>
+  <si>
     <t>SICTHS39NBF</t>
   </si>
   <si>
     <t>SECTION;HAT;TABLETOP;39;NBF</t>
   </si>
   <si>
+    <t>LOADED</t>
+  </si>
+  <si>
+    <t>SIZCLMNBF</t>
+  </si>
+  <si>
+    <t>ASM;BASE;COLUMN;4IN;NBF</t>
+  </si>
+  <si>
     <t>HARDWARE PACKING</t>
   </si>
   <si>
-    <t>MATERIAL</t>
-  </si>
-  <si>
     <t>382905K</t>
   </si>
   <si>
     <t>SECT;HAT;TABLETOP;38.724IN;K</t>
   </si>
   <si>
-    <t>EA</t>
-  </si>
-  <si>
-    <t>Work Instruction</t>
-  </si>
-  <si>
     <t>INS496</t>
   </si>
   <si>
@@ -123,12 +225,6 @@
     <t>FST</t>
   </si>
   <si>
-    <t>SIZCLMNBF</t>
-  </si>
-  <si>
-    <t>ASM;BASE;COLUMN;4IN;NBF</t>
-  </si>
-  <si>
     <t>LEG / BASE PACKING</t>
   </si>
   <si>
@@ -144,105 +240,9 @@
     <t>SUPPORT;TABLE;4IN;PA</t>
   </si>
   <si>
-    <t>KIT;HDWE;SCREW;BASE;TFL</t>
-  </si>
-  <si>
     <t>PAD;DIE CUT;LEG FILLER;TRIG;11 X 6</t>
   </si>
   <si>
-    <t>SIZRECT48STRCLMNBF</t>
-  </si>
-  <si>
-    <t>TOP;RECT;CLM;STR;48X48;NBF</t>
-  </si>
-  <si>
-    <t>FS SAWS A &amp; B</t>
-  </si>
-  <si>
-    <t>810510-XZM</t>
-  </si>
-  <si>
-    <t>TFM;XZM;1.0X5X10-LIGHT GRAY</t>
-  </si>
-  <si>
-    <t>SF</t>
-  </si>
-  <si>
-    <t>A2 CUT 48.3960 X 48.3960  GRAIN 0CUT TO ROUGH SIZE</t>
-  </si>
-  <si>
-    <t>FS ROUTERS</t>
-  </si>
-  <si>
-    <t>FS EDGEBAND/BOX</t>
-  </si>
-  <si>
-    <t>(EXP)BLOCK;WS;SIDE FILLER</t>
-  </si>
-  <si>
-    <t>SEND TO 5209 FOR NBF PACKAGE LABEL</t>
-  </si>
-  <si>
-    <t>387880XZM</t>
-  </si>
-  <si>
-    <t>EDGEBAND;PVC;1.125X.118 IN;XZM</t>
-  </si>
-  <si>
-    <t>FT</t>
-  </si>
-  <si>
-    <t>(EXP)BOX;TOP;WS;58.75 X 50.375 X 1.25</t>
-  </si>
-  <si>
-    <t>(EXP)BOX;BTM;WS;58.75 X 50.375 X 1.25</t>
-  </si>
-  <si>
-    <t>(EXP)END;BOX;WS;50.25 X 1.25 IN</t>
-  </si>
-  <si>
-    <t>LABEL;NBF;STICK ON</t>
-  </si>
-  <si>
-    <t>INTRINSIC ACCES/SERV</t>
-  </si>
-  <si>
-    <t>LABEL;PACKAGE;NBF;11 X 8.5</t>
-  </si>
-  <si>
-    <t>ATTACH NBF PACKAGE LABEL</t>
-  </si>
-  <si>
-    <t>PACK TABLES 99 PACK</t>
-  </si>
-  <si>
-    <t>CONNECTOR;TABLETOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>252794K</t>
-  </si>
-  <si>
-    <t>PLATE;SPPT;TABLE;6X3.5;K</t>
-  </si>
-  <si>
-    <t>SIZRECTSTRNBF</t>
-  </si>
-  <si>
-    <t>NBF40962;TABLE;RECT;STR;48X48</t>
-  </si>
-  <si>
-    <t>PARENT KNOCK DOWN WC</t>
-  </si>
-  <si>
-    <t>TKD</t>
-  </si>
-  <si>
-    <t>LOADED</t>
-  </si>
-  <si>
     <t>SIZRECT48MIDCLMNBF</t>
   </si>
   <si>
@@ -256,18 +256,6 @@
   </si>
   <si>
     <t>NBF40960;TABLE;RECT;MID;48X48</t>
-  </si>
-  <si>
-    <t>SIZRECTENDNBF</t>
-  </si>
-  <si>
-    <t>NBF40964;TABLE;RECT;END;48X48</t>
-  </si>
-  <si>
-    <t>SIZRECT48ENDCLMNBF</t>
-  </si>
-  <si>
-    <t>TOP;RECT;CLM;END;48X48;NBF</t>
   </si>
 </sst>
 </file>
@@ -633,16 +621,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A438DC8-B175-4B7F-A9E5-7EF1556A379D}">
-  <dimension ref="A1:R60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C2EB49-7817-4366-A18C-7FB8D0256835}">
+  <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -698,7 +686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -719,7 +707,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="3">
-        <v>7203</v>
+        <v>2806</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>22</v>
@@ -734,21 +722,23 @@
         <v>24</v>
       </c>
       <c r="M2" s="3">
-        <v>1</v>
+        <v>23.08681</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="O2" s="3">
-        <v>7201</v>
+        <v>2807</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -763,42 +753,30 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H3" s="3">
-        <v>7203</v>
+        <v>2803</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="3">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="3">
-        <v>1</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="3">
-        <v>7201</v>
-      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -813,42 +791,44 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H4" s="3">
-        <v>7203</v>
+        <v>2807</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="3">
-        <v>3</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>29</v>
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>319112</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="M4" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="O4" s="3">
+        <v>2807</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -856,51 +836,51 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2807</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="3">
-        <v>6309</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>371157</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3">
+        <v>11.986000000000001</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="3">
-        <v>1</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>31</v>
+      <c r="O5" s="3">
+        <v>2807</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -908,51 +888,51 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H6" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="3">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>37</v>
+        <v>3</v>
+      </c>
+      <c r="K6" s="3">
+        <v>400511</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O6" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -960,51 +940,51 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H7" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K7" s="3">
-        <v>392331</v>
+        <v>400517</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O7" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1012,51 +992,51 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H8" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K8" s="3">
-        <v>393550</v>
+        <v>400527</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O8" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1064,38 +1044,38 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H9" s="3">
-        <v>2806</v>
+        <v>2807</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="3">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
+      </c>
+      <c r="K9" s="3">
+        <v>404058</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M9" s="3">
-        <v>23.08681</v>
+        <v>1</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="O9" s="3">
         <v>2807</v>
@@ -1105,10 +1085,10 @@
         <v>26</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1116,37 +1096,51 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="3">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H10" s="3">
-        <v>2803</v>
+        <v>5209</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>404059</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="3">
+        <v>5209</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1154,20 +1148,20 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H11" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>22</v>
@@ -1176,29 +1170,27 @@
         <v>1</v>
       </c>
       <c r="K11" s="3">
-        <v>319112</v>
+        <v>252786</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M11" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O11" s="3">
-        <v>2807</v>
+        <v>31</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R11" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -1206,20 +1198,20 @@
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H12" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>22</v>
@@ -1228,29 +1220,27 @@
         <v>2</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="M12" s="3">
-        <v>11.986000000000001</v>
+        <v>2</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="O12" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R12" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -1258,20 +1248,20 @@
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H13" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>22</v>
@@ -1280,29 +1270,27 @@
         <v>3</v>
       </c>
       <c r="K13" s="3">
-        <v>400511</v>
+        <v>392331</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="M13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O13" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R13" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -1310,103 +1298,103 @@
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P14" s="3">
+        <v>1051</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="3">
-        <v>2807</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="3">
-        <v>4</v>
-      </c>
-      <c r="K14" s="3">
-        <v>400517</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M14" s="3">
-        <v>0</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O14" s="3">
-        <v>2807</v>
-      </c>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="3">
-        <v>2807</v>
+        <v>51</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="3">
-        <v>5</v>
-      </c>
-      <c r="K15" s="3">
-        <v>400527</v>
+        <v>2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>57</v>
       </c>
       <c r="M15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O15" s="3">
-        <v>2807</v>
-      </c>
-      <c r="P15" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P15" s="3">
+        <v>1051</v>
+      </c>
       <c r="Q15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1414,51 +1402,51 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="3">
-        <v>2807</v>
+        <v>51</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J16" s="3">
-        <v>6</v>
-      </c>
-      <c r="K16" s="3">
-        <v>404058</v>
+        <v>3</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="M16" s="3">
         <v>1</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O16" s="3">
-        <v>2807</v>
-      </c>
-      <c r="P16" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P16" s="3">
+        <v>1051</v>
+      </c>
       <c r="Q16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R16" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1466,29 +1454,29 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="3">
+        <v>7203</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="H17" s="3">
-        <v>5209</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="3">
-        <v>1</v>
-      </c>
-      <c r="K17" s="3">
-        <v>404059</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>60</v>
@@ -1497,20 +1485,18 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O17" s="3">
-        <v>5209</v>
+        <v>7201</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -1518,41 +1504,41 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="3">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="3">
+        <v>7203</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="3">
+      <c r="M18" s="3">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18" s="3">
         <v>7201</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="3">
-        <v>1</v>
-      </c>
-      <c r="K18" s="3">
-        <v>252786</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="M18" s="3">
-        <v>4</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="3" t="s">
@@ -1560,7 +1546,7 @@
       </c>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1568,41 +1554,41 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="3">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H19" s="3">
-        <v>7201</v>
+        <v>7203</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J19" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="M19" s="3">
+        <v>10</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M19" s="3">
-        <v>2</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O19" s="3">
-        <v>5209</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="3" t="s">
@@ -1610,7 +1596,7 @@
       </c>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1618,49 +1604,51 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="3">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H20" s="3">
-        <v>7201</v>
+        <v>6309</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K20" s="3">
-        <v>392331</v>
+        <v>371157</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="M20" s="3">
         <v>1</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O20" s="3">
-        <v>5209</v>
+        <v>31</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R20" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -1668,51 +1656,51 @@
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="3">
+        <v>6309</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="3">
+        <v>2</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="3">
-        <v>1</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="M21" s="3">
         <v>1</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P21" s="3">
-        <v>1051</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="O21" s="3">
+        <v>6309</v>
+      </c>
+      <c r="P21" s="1"/>
       <c r="Q21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R21" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -1720,51 +1708,51 @@
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="H22" s="3">
+        <v>6309</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J22" s="3">
-        <v>2</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>32</v>
+        <v>3</v>
+      </c>
+      <c r="K22" s="3">
+        <v>392331</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="M22" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P22" s="3">
-        <v>1051</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="O22" s="3">
+        <v>6309</v>
+      </c>
+      <c r="P22" s="1"/>
       <c r="Q22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R22" s="1"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R22" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
@@ -1772,51 +1760,51 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="H23" s="3">
+        <v>6309</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J23" s="3">
-        <v>3</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>41</v>
+        <v>4</v>
+      </c>
+      <c r="K23" s="3">
+        <v>393550</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="M23" s="3">
         <v>1</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P23" s="3">
-        <v>1051</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="O23" s="3">
+        <v>6309</v>
+      </c>
+      <c r="P23" s="1"/>
       <c r="Q23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
@@ -1824,20 +1812,20 @@
         <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="3">
         <v>10</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H24" s="3">
-        <v>6309</v>
+        <v>2806</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>22</v>
@@ -1845,30 +1833,30 @@
       <c r="J24" s="3">
         <v>1</v>
       </c>
-      <c r="K24" s="3">
-        <v>371157</v>
+      <c r="K24" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="M24" s="3">
-        <v>1</v>
+        <v>23.08681</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>31</v>
+      <c r="O24" s="3">
+        <v>2807</v>
       </c>
       <c r="P24" s="1"/>
       <c r="Q24" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
@@ -1876,51 +1864,37 @@
         <v>2</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H25" s="3">
-        <v>6309</v>
+        <v>2803</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="3">
-        <v>2</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M25" s="3">
-        <v>1</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O25" s="3">
-        <v>6309</v>
-      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R25" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
@@ -1928,51 +1902,51 @@
         <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H26" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J26" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K26" s="3">
-        <v>392331</v>
+        <v>319112</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="M26" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O26" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>18</v>
       </c>
@@ -1980,51 +1954,51 @@
         <v>2</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="3">
+        <v>2807</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="3">
-        <v>6309</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J27" s="3">
-        <v>4</v>
-      </c>
-      <c r="K27" s="3">
-        <v>393550</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="M27" s="3">
-        <v>1</v>
+        <v>11.986000000000001</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="O27" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>18</v>
       </c>
@@ -2039,31 +2013,31 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H28" s="3">
-        <v>2806</v>
+        <v>2807</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J28" s="3">
-        <v>1</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="K28" s="3">
+        <v>400511</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="M28" s="3">
-        <v>23.08681</v>
+        <v>0</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="O28" s="3">
         <v>2807</v>
@@ -2073,10 +2047,10 @@
         <v>26</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>18</v>
       </c>
@@ -2091,30 +2065,44 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="H29" s="3">
-        <v>2803</v>
+        <v>2807</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
+      <c r="J29" s="3">
+        <v>4</v>
+      </c>
+      <c r="K29" s="3">
+        <v>400517</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O29" s="3">
+        <v>2807</v>
+      </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R29" s="1"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R29" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
@@ -2132,7 +2120,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="H30" s="3">
         <v>2807</v>
@@ -2141,19 +2129,19 @@
         <v>22</v>
       </c>
       <c r="J30" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K30" s="3">
-        <v>319112</v>
+        <v>400527</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="M30" s="3">
         <v>0</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O30" s="3">
         <v>2807</v>
@@ -2166,7 +2154,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
@@ -2184,7 +2172,7 @@
         <v>30</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="H31" s="3">
         <v>2807</v>
@@ -2193,19 +2181,19 @@
         <v>22</v>
       </c>
       <c r="J31" s="3">
-        <v>2</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>52</v>
+        <v>6</v>
+      </c>
+      <c r="K31" s="3">
+        <v>404058</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="M31" s="3">
-        <v>11.986000000000001</v>
+        <v>1</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="O31" s="3">
         <v>2807</v>
@@ -2218,7 +2206,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
@@ -2233,44 +2221,44 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="3">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H32" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J32" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K32" s="3">
-        <v>400511</v>
+        <v>404059</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="M32" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O32" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
@@ -2285,44 +2273,42 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H33" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J33" s="3">
+        <v>1</v>
+      </c>
+      <c r="K33" s="3">
+        <v>252786</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M33" s="3">
         <v>4</v>
       </c>
-      <c r="K33" s="3">
-        <v>400517</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M33" s="3">
-        <v>0</v>
-      </c>
       <c r="N33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O33" s="3">
-        <v>2807</v>
+        <v>31</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="P33" s="1"/>
       <c r="Q33" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R33" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
@@ -2337,44 +2323,42 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H34" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="3">
-        <v>5</v>
-      </c>
-      <c r="K34" s="3">
-        <v>400527</v>
+        <v>2</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M34" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O34" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R34" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
@@ -2389,44 +2373,42 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H35" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J35" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K35" s="3">
-        <v>404058</v>
+        <v>392331</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="M35" s="3">
         <v>1</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O35" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R35" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R35" s="1"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
@@ -2434,20 +2416,20 @@
         <v>2</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="3">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H36" s="3">
-        <v>5209</v>
+        <v>51</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>22</v>
@@ -2455,30 +2437,30 @@
       <c r="J36" s="3">
         <v>1</v>
       </c>
-      <c r="K36" s="3">
-        <v>404059</v>
+      <c r="K36" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="M36" s="3">
         <v>1</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O36" s="3">
-        <v>5209</v>
-      </c>
-      <c r="P36" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P36" s="3">
+        <v>1051</v>
+      </c>
       <c r="Q36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R36" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R36" s="1"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
@@ -2486,49 +2468,51 @@
         <v>2</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="3">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H37" s="3">
-        <v>7201</v>
+        <v>51</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J37" s="3">
-        <v>1</v>
-      </c>
-      <c r="K37" s="3">
-        <v>252786</v>
+        <v>2</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="M37" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="P37" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="P37" s="3">
+        <v>1051</v>
+      </c>
       <c r="Q37" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>18</v>
       </c>
@@ -2536,49 +2520,51 @@
         <v>2</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="3">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H38" s="3">
-        <v>7201</v>
+        <v>51</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J38" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="M38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O38" s="3">
-        <v>5209</v>
-      </c>
-      <c r="P38" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P38" s="3">
+        <v>1051</v>
+      </c>
       <c r="Q38" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>18</v>
       </c>
@@ -2586,41 +2572,41 @@
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="3">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H39" s="3">
+        <v>7203</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="3">
+        <v>1</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M39" s="3">
+        <v>1</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O39" s="3">
         <v>7201</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J39" s="3">
-        <v>3</v>
-      </c>
-      <c r="K39" s="3">
-        <v>392331</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M39" s="3">
-        <v>1</v>
-      </c>
-      <c r="N39" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O39" s="3">
-        <v>5209</v>
       </c>
       <c r="P39" s="1"/>
       <c r="Q39" s="3" t="s">
@@ -2628,7 +2614,7 @@
       </c>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
@@ -2636,51 +2622,49 @@
         <v>2</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
+      </c>
+      <c r="H40" s="3">
+        <v>7203</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J40" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="M40" s="3">
         <v>1</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O40" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P40" s="3">
-        <v>1051</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="O40" s="3">
+        <v>7201</v>
+      </c>
+      <c r="P40" s="1"/>
       <c r="Q40" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
@@ -2688,51 +2672,49 @@
         <v>2</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
+      </c>
+      <c r="H41" s="3">
+        <v>7203</v>
       </c>
       <c r="I41" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J41" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="M41" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P41" s="3">
-        <v>1051</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="P41" s="1"/>
       <c r="Q41" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>18</v>
       </c>
@@ -2740,51 +2722,51 @@
         <v>2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="H42" s="3">
+        <v>6309</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J42" s="3">
-        <v>3</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>72</v>
+        <v>1</v>
+      </c>
+      <c r="K42" s="3">
+        <v>371157</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="M42" s="3">
         <v>1</v>
       </c>
       <c r="N42" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P42" s="3">
-        <v>1051</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="P42" s="1"/>
       <c r="Q42" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R42" s="1"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R42" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>18</v>
       </c>
@@ -2792,49 +2774,51 @@
         <v>2</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="3">
         <v>10</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="H43" s="3">
-        <v>7203</v>
+        <v>6309</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J43" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="M43" s="3">
         <v>1</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O43" s="3">
-        <v>7201</v>
+        <v>6309</v>
       </c>
       <c r="P43" s="1"/>
       <c r="Q43" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R43" s="1"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R43" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>18</v>
       </c>
@@ -2842,49 +2826,51 @@
         <v>2</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="3">
         <v>10</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="H44" s="3">
-        <v>7203</v>
+        <v>6309</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J44" s="3">
-        <v>2</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="K44" s="3">
+        <v>392331</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="M44" s="3">
         <v>1</v>
       </c>
       <c r="N44" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O44" s="3">
-        <v>7201</v>
+        <v>6309</v>
       </c>
       <c r="P44" s="1"/>
       <c r="Q44" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R44" s="1"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R44" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>18</v>
       </c>
@@ -2892,49 +2878,51 @@
         <v>2</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="3">
         <v>10</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="H45" s="3">
-        <v>7203</v>
+        <v>6309</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J45" s="3">
-        <v>3</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>29</v>
+        <v>4</v>
+      </c>
+      <c r="K45" s="3">
+        <v>393550</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="M45" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O45" s="3" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="O45" s="3">
+        <v>6309</v>
       </c>
       <c r="P45" s="1"/>
       <c r="Q45" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R45" s="1"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R45" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>18</v>
       </c>
@@ -2942,20 +2930,20 @@
         <v>3</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>70</v>
+        <v>21</v>
+      </c>
+      <c r="H46" s="3">
+        <v>2806</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>22</v>
@@ -2964,29 +2952,29 @@
         <v>1</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="M46" s="3">
-        <v>2</v>
+        <v>23.08681</v>
       </c>
       <c r="N46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O46" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P46" s="3">
-        <v>857</v>
-      </c>
+      <c r="O46" s="3">
+        <v>2807</v>
+      </c>
+      <c r="P46" s="1"/>
       <c r="Q46" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R46" s="1"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R46" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>18</v>
       </c>
@@ -2994,51 +2982,37 @@
         <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>70</v>
+        <v>28</v>
+      </c>
+      <c r="H47" s="3">
+        <v>2803</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J47" s="3">
-        <v>2</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L47" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M47" s="3">
-        <v>1</v>
-      </c>
-      <c r="N47" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O47" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P47" s="3">
-        <v>857</v>
-      </c>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
       <c r="Q47" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>18</v>
       </c>
@@ -3046,20 +3020,20 @@
         <v>3</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H48" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>22</v>
@@ -3068,29 +3042,29 @@
         <v>1</v>
       </c>
       <c r="K48" s="3">
-        <v>371157</v>
+        <v>319112</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M48" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N48" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O48" s="3" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="O48" s="3">
+        <v>2807</v>
       </c>
       <c r="P48" s="1"/>
       <c r="Q48" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>18</v>
       </c>
@@ -3098,51 +3072,51 @@
         <v>3</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" s="3">
+        <v>2807</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J49" s="3">
+        <v>2</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L49" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H49" s="3">
-        <v>6309</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J49" s="3">
-        <v>2</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="M49" s="3">
-        <v>1</v>
+        <v>11.986000000000001</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="O49" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="P49" s="1"/>
       <c r="Q49" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
@@ -3150,20 +3124,20 @@
         <v>3</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H50" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>22</v>
@@ -3172,29 +3146,29 @@
         <v>3</v>
       </c>
       <c r="K50" s="3">
-        <v>392331</v>
+        <v>400511</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M50" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O50" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="P50" s="1"/>
       <c r="Q50" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R50" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>18</v>
       </c>
@@ -3202,20 +3176,20 @@
         <v>3</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H51" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>22</v>
@@ -3224,29 +3198,29 @@
         <v>4</v>
       </c>
       <c r="K51" s="3">
-        <v>393550</v>
+        <v>400517</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M51" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O51" s="3">
-        <v>6309</v>
+        <v>2807</v>
       </c>
       <c r="P51" s="1"/>
       <c r="Q51" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R51" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>18</v>
       </c>
@@ -3254,38 +3228,38 @@
         <v>3</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H52" s="3">
-        <v>2806</v>
+        <v>2807</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J52" s="3">
-        <v>1</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>44</v>
+        <v>5</v>
+      </c>
+      <c r="K52" s="3">
+        <v>400527</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="M52" s="3">
-        <v>23.08681</v>
+        <v>0</v>
       </c>
       <c r="N52" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="O52" s="3">
         <v>2807</v>
@@ -3295,10 +3269,10 @@
         <v>26</v>
       </c>
       <c r="R52" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>18</v>
       </c>
@@ -3306,37 +3280,51 @@
         <v>3</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="H53" s="3">
-        <v>2803</v>
+        <v>2807</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
+      <c r="J53" s="3">
+        <v>6</v>
+      </c>
+      <c r="K53" s="3">
+        <v>404058</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M53" s="3">
+        <v>1</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O53" s="3">
+        <v>2807</v>
+      </c>
       <c r="P53" s="1"/>
       <c r="Q53" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R53" s="1"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R53" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>18</v>
       </c>
@@ -3344,20 +3332,20 @@
         <v>3</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="3">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H54" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>22</v>
@@ -3366,29 +3354,29 @@
         <v>1</v>
       </c>
       <c r="K54" s="3">
-        <v>319112</v>
+        <v>404059</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="M54" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O54" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="P54" s="1"/>
       <c r="Q54" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>18</v>
       </c>
@@ -3396,51 +3384,49 @@
         <v>3</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H55" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J55" s="3">
-        <v>2</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>52</v>
+        <v>1</v>
+      </c>
+      <c r="K55" s="3">
+        <v>252786</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="M55" s="3">
-        <v>11.986000000000001</v>
+        <v>4</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O55" s="3">
-        <v>2807</v>
+        <v>31</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="P55" s="1"/>
       <c r="Q55" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R55" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R55" s="1"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>18</v>
       </c>
@@ -3448,51 +3434,49 @@
         <v>3</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H56" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J56" s="3">
-        <v>3</v>
-      </c>
-      <c r="K56" s="3">
-        <v>400511</v>
+        <v>2</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="M56" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N56" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O56" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="P56" s="1"/>
       <c r="Q56" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R56" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R56" s="1"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>18</v>
       </c>
@@ -3500,51 +3484,49 @@
         <v>3</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H57" s="3">
-        <v>2807</v>
+        <v>7201</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J57" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K57" s="3">
-        <v>400517</v>
+        <v>392331</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="M57" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N57" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O57" s="3">
-        <v>2807</v>
+        <v>5209</v>
       </c>
       <c r="P57" s="1"/>
       <c r="Q57" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R57" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R57" s="1"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>18</v>
       </c>
@@ -3552,51 +3534,51 @@
         <v>3</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H58" s="3">
-        <v>2807</v>
+        <v>51</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J58" s="3">
-        <v>5</v>
-      </c>
-      <c r="K58" s="3">
-        <v>400527</v>
+        <v>1</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M58" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O58" s="3">
-        <v>2807</v>
-      </c>
-      <c r="P58" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P58" s="3">
+        <v>1051</v>
+      </c>
       <c r="Q58" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R58" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R58" s="1"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>18</v>
       </c>
@@ -3604,51 +3586,51 @@
         <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H59" s="3">
-        <v>2807</v>
+        <v>51</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J59" s="3">
-        <v>6</v>
-      </c>
-      <c r="K59" s="3">
-        <v>404058</v>
+        <v>2</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M59" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N59" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O59" s="3">
-        <v>2807</v>
-      </c>
-      <c r="P59" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P59" s="3">
+        <v>1051</v>
+      </c>
       <c r="Q59" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R59" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R59" s="1"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>18</v>
       </c>
@@ -3656,51 +3638,639 @@
         <v>3</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="3">
+        <v>1</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J60" s="3">
+        <v>3</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M60" s="3">
+        <v>1</v>
+      </c>
+      <c r="N60" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O60" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P60" s="3">
+        <v>1051</v>
+      </c>
+      <c r="Q60" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R60" s="1"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="3">
+        <v>3</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="3">
+        <v>10</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H61" s="3">
+        <v>7203</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J61" s="3">
+        <v>1</v>
+      </c>
+      <c r="K61" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M61" s="3">
+        <v>1</v>
+      </c>
+      <c r="N61" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O61" s="3">
+        <v>7201</v>
+      </c>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R61" s="1"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="3">
+        <v>3</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="3">
+        <v>10</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H62" s="3">
+        <v>7203</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J62" s="3">
+        <v>2</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M62" s="3">
+        <v>1</v>
+      </c>
+      <c r="N62" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O62" s="3">
+        <v>7201</v>
+      </c>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R62" s="1"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" s="3">
+        <v>3</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="3">
+        <v>10</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H63" s="3">
+        <v>7203</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J63" s="3">
+        <v>3</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="M63" s="3">
+        <v>10</v>
+      </c>
+      <c r="N63" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O63" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R63" s="1"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="3">
+        <v>3</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="3">
+        <v>10</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H64" s="3">
+        <v>6309</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J64" s="3">
+        <v>1</v>
+      </c>
+      <c r="K64" s="3">
+        <v>371157</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M64" s="3">
+        <v>1</v>
+      </c>
+      <c r="N64" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O64" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R64" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="3">
+        <v>3</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="3">
+        <v>10</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H65" s="3">
+        <v>6309</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J65" s="3">
+        <v>2</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L65" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G60" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H60" s="3">
-        <v>5209</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J60" s="3">
-        <v>1</v>
-      </c>
-      <c r="K60" s="3">
-        <v>404059</v>
-      </c>
-      <c r="L60" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="M60" s="3">
-        <v>1</v>
-      </c>
-      <c r="N60" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O60" s="3">
-        <v>5209</v>
-      </c>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R60" s="3" t="s">
-        <v>61</v>
+      <c r="M65" s="3">
+        <v>1</v>
+      </c>
+      <c r="N65" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O65" s="3">
+        <v>6309</v>
+      </c>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R65" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="3">
+        <v>3</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="3">
+        <v>10</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H66" s="3">
+        <v>6309</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J66" s="3">
+        <v>3</v>
+      </c>
+      <c r="K66" s="3">
+        <v>392331</v>
+      </c>
+      <c r="L66" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M66" s="3">
+        <v>1</v>
+      </c>
+      <c r="N66" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O66" s="3">
+        <v>6309</v>
+      </c>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="3">
+        <v>3</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="3">
+        <v>10</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H67" s="3">
+        <v>6309</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J67" s="3">
+        <v>4</v>
+      </c>
+      <c r="K67" s="3">
+        <v>393550</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M67" s="3">
+        <v>1</v>
+      </c>
+      <c r="N67" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O67" s="3">
+        <v>6309</v>
+      </c>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R67" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010092D94451A280D548907CBCF1F281E270" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4978586239b112e43b317771f22ec7c5">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="81ea7e4c-c175-424d-a668-f1797cbc8752" xmlns:ns3="a3e5204a-12c1-4e5c-8776-9a11a94c075a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb8e97fce5598dd36bb5089d07f307e7" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="81ea7e4c-c175-424d-a668-f1797cbc8752"/>
+    <xsd:import namespace="a3e5204a-12c1-4e5c-8776-9a11a94c075a"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="12" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="13" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="81ea7e4c-c175-424d-a668-f1797cbc8752" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="16" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a3e5204a-12c1-4e5c-8776-9a11a94c075a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B175CFCC-63A9-4563-A353-E517DBCE10FE}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0E2621-4CC1-4D53-9555-EF6CCCA0E77A}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8F6C528-E31A-4ABE-934E-D8669434E239}"/>
 </file>
</xml_diff>